<commit_message>
Correccion error IDE 010503
</commit_message>
<xml_diff>
--- a/Catalogo_Normalizado.xlsx
+++ b/Catalogo_Normalizado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\MejoraCatalogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF06E83-EBCF-498E-9D12-182172A8E5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5161859-C8A5-470D-9F21-261F150297A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="145" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7222" uniqueCount="3071">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7226" uniqueCount="3071">
   <si>
     <t xml:space="preserve">CATÁLOGO DE OBJETOS GEOGRÁFICOS DE LA INFRAESTRUCTURA DE DATOS ESPACIALES DE LA PROVINCIA DE TIERRA DEL FUEGO AeIAS </t>
   </si>
@@ -12077,24 +12077,19 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="68" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -12103,52 +12098,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -12164,8 +12125,84 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -12196,43 +12233,6 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -12988,418 +12988,440 @@
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="243" t="s">
+      <c r="A1" s="286" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="244"/>
-      <c r="C1" s="244"/>
-      <c r="D1" s="244"/>
-      <c r="E1" s="244"/>
-      <c r="F1" s="244"/>
-      <c r="G1" s="244"/>
-      <c r="H1" s="244"/>
-      <c r="I1" s="244"/>
-      <c r="J1" s="244"/>
-      <c r="K1" s="244"/>
-      <c r="L1" s="244"/>
-      <c r="M1" s="244"/>
-      <c r="N1" s="244"/>
-      <c r="O1" s="245"/>
+      <c r="B1" s="281"/>
+      <c r="C1" s="281"/>
+      <c r="D1" s="281"/>
+      <c r="E1" s="281"/>
+      <c r="F1" s="281"/>
+      <c r="G1" s="281"/>
+      <c r="H1" s="281"/>
+      <c r="I1" s="281"/>
+      <c r="J1" s="281"/>
+      <c r="K1" s="281"/>
+      <c r="L1" s="281"/>
+      <c r="M1" s="281"/>
+      <c r="N1" s="281"/>
+      <c r="O1" s="272"/>
     </row>
     <row r="2" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="246" t="s">
+      <c r="A2" s="280" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="244"/>
-      <c r="C2" s="247"/>
-      <c r="D2" s="248" t="s">
+      <c r="B2" s="281"/>
+      <c r="C2" s="282"/>
+      <c r="D2" s="287" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
-      <c r="H2" s="244"/>
-      <c r="I2" s="244"/>
-      <c r="J2" s="244"/>
-      <c r="K2" s="244"/>
-      <c r="L2" s="244"/>
-      <c r="M2" s="244"/>
-      <c r="N2" s="244"/>
-      <c r="O2" s="245"/>
+      <c r="E2" s="281"/>
+      <c r="F2" s="281"/>
+      <c r="G2" s="281"/>
+      <c r="H2" s="281"/>
+      <c r="I2" s="281"/>
+      <c r="J2" s="281"/>
+      <c r="K2" s="281"/>
+      <c r="L2" s="281"/>
+      <c r="M2" s="281"/>
+      <c r="N2" s="281"/>
+      <c r="O2" s="272"/>
     </row>
     <row r="3" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="246" t="s">
+      <c r="A3" s="280" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="244"/>
-      <c r="C3" s="247"/>
-      <c r="D3" s="249" t="s">
+      <c r="B3" s="281"/>
+      <c r="C3" s="282"/>
+      <c r="D3" s="288" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="244"/>
-      <c r="F3" s="244"/>
-      <c r="G3" s="244"/>
-      <c r="H3" s="244"/>
-      <c r="I3" s="244"/>
-      <c r="J3" s="244"/>
-      <c r="K3" s="244"/>
-      <c r="L3" s="244"/>
-      <c r="M3" s="244"/>
-      <c r="N3" s="244"/>
-      <c r="O3" s="245"/>
+      <c r="E3" s="281"/>
+      <c r="F3" s="281"/>
+      <c r="G3" s="281"/>
+      <c r="H3" s="281"/>
+      <c r="I3" s="281"/>
+      <c r="J3" s="281"/>
+      <c r="K3" s="281"/>
+      <c r="L3" s="281"/>
+      <c r="M3" s="281"/>
+      <c r="N3" s="281"/>
+      <c r="O3" s="272"/>
     </row>
     <row r="4" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="246" t="s">
+      <c r="A4" s="280" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="244"/>
-      <c r="C4" s="247"/>
-      <c r="D4" s="272" t="s">
+      <c r="B4" s="281"/>
+      <c r="C4" s="282"/>
+      <c r="D4" s="283" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="244"/>
-      <c r="F4" s="247"/>
-      <c r="G4" s="273" t="s">
+      <c r="E4" s="281"/>
+      <c r="F4" s="282"/>
+      <c r="G4" s="284" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="247"/>
-      <c r="I4" s="274" t="s">
+      <c r="H4" s="282"/>
+      <c r="I4" s="285" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="244"/>
-      <c r="K4" s="247"/>
-      <c r="L4" s="273" t="s">
+      <c r="J4" s="281"/>
+      <c r="K4" s="282"/>
+      <c r="L4" s="284" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="247"/>
-      <c r="N4" s="250" t="s">
+      <c r="M4" s="282"/>
+      <c r="N4" s="271" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="245"/>
+      <c r="O4" s="272"/>
     </row>
     <row r="5" spans="1:15" ht="13" x14ac:dyDescent="0.25">
-      <c r="A5" s="251" t="s">
+      <c r="A5" s="250" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="252"/>
-      <c r="C5" s="253"/>
-      <c r="D5" s="260" t="s">
+      <c r="B5" s="251"/>
+      <c r="C5" s="252"/>
+      <c r="D5" s="274" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="261"/>
-      <c r="F5" s="261"/>
-      <c r="G5" s="261"/>
-      <c r="H5" s="261"/>
-      <c r="I5" s="261"/>
-      <c r="J5" s="261"/>
-      <c r="K5" s="262"/>
+      <c r="E5" s="275"/>
+      <c r="F5" s="275"/>
+      <c r="G5" s="275"/>
+      <c r="H5" s="275"/>
+      <c r="I5" s="275"/>
+      <c r="J5" s="275"/>
+      <c r="K5" s="276"/>
       <c r="L5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="263" t="s">
+      <c r="M5" s="277" t="s">
         <v>14</v>
       </c>
-      <c r="N5" s="264"/>
-      <c r="O5" s="265"/>
+      <c r="N5" s="260"/>
+      <c r="O5" s="261"/>
     </row>
     <row r="6" spans="1:15" ht="13" x14ac:dyDescent="0.25">
-      <c r="A6" s="254"/>
-      <c r="B6" s="255"/>
-      <c r="C6" s="256"/>
-      <c r="D6" s="266" t="s">
+      <c r="A6" s="253"/>
+      <c r="B6" s="254"/>
+      <c r="C6" s="255"/>
+      <c r="D6" s="278" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="267"/>
-      <c r="F6" s="267"/>
-      <c r="G6" s="267"/>
-      <c r="H6" s="267"/>
-      <c r="I6" s="267"/>
-      <c r="J6" s="267"/>
-      <c r="K6" s="268"/>
+      <c r="E6" s="244"/>
+      <c r="F6" s="244"/>
+      <c r="G6" s="244"/>
+      <c r="H6" s="244"/>
+      <c r="I6" s="244"/>
+      <c r="J6" s="244"/>
+      <c r="K6" s="263"/>
       <c r="L6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="269" t="s">
+      <c r="M6" s="279" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="267"/>
-      <c r="O6" s="270"/>
+      <c r="N6" s="244"/>
+      <c r="O6" s="245"/>
     </row>
     <row r="7" spans="1:15" ht="13" x14ac:dyDescent="0.25">
-      <c r="A7" s="254"/>
-      <c r="B7" s="255"/>
-      <c r="C7" s="256"/>
-      <c r="D7" s="266" t="s">
+      <c r="A7" s="253"/>
+      <c r="B7" s="254"/>
+      <c r="C7" s="255"/>
+      <c r="D7" s="278" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="267"/>
-      <c r="F7" s="267"/>
-      <c r="G7" s="267"/>
-      <c r="H7" s="267"/>
-      <c r="I7" s="267"/>
-      <c r="J7" s="267"/>
-      <c r="K7" s="268"/>
+      <c r="E7" s="244"/>
+      <c r="F7" s="244"/>
+      <c r="G7" s="244"/>
+      <c r="H7" s="244"/>
+      <c r="I7" s="244"/>
+      <c r="J7" s="244"/>
+      <c r="K7" s="263"/>
       <c r="L7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="271" t="s">
+      <c r="M7" s="246" t="s">
         <v>18</v>
       </c>
-      <c r="N7" s="267"/>
-      <c r="O7" s="270"/>
+      <c r="N7" s="244"/>
+      <c r="O7" s="245"/>
     </row>
     <row r="8" spans="1:15" ht="13" x14ac:dyDescent="0.25">
-      <c r="A8" s="254"/>
-      <c r="B8" s="255"/>
-      <c r="C8" s="256"/>
-      <c r="D8" s="266" t="s">
+      <c r="A8" s="253"/>
+      <c r="B8" s="254"/>
+      <c r="C8" s="255"/>
+      <c r="D8" s="278" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="267"/>
-      <c r="F8" s="267"/>
-      <c r="G8" s="267"/>
-      <c r="H8" s="267"/>
-      <c r="I8" s="267"/>
-      <c r="J8" s="267"/>
-      <c r="K8" s="268"/>
+      <c r="E8" s="244"/>
+      <c r="F8" s="244"/>
+      <c r="G8" s="244"/>
+      <c r="H8" s="244"/>
+      <c r="I8" s="244"/>
+      <c r="J8" s="244"/>
+      <c r="K8" s="263"/>
       <c r="L8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="269" t="s">
+      <c r="M8" s="279" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="267"/>
-      <c r="O8" s="270"/>
+      <c r="N8" s="244"/>
+      <c r="O8" s="245"/>
     </row>
     <row r="9" spans="1:15" ht="13" x14ac:dyDescent="0.25">
-      <c r="A9" s="254"/>
-      <c r="B9" s="255"/>
-      <c r="C9" s="256"/>
-      <c r="D9" s="266" t="s">
+      <c r="A9" s="253"/>
+      <c r="B9" s="254"/>
+      <c r="C9" s="255"/>
+      <c r="D9" s="278" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="267"/>
-      <c r="F9" s="267"/>
-      <c r="G9" s="267"/>
-      <c r="H9" s="267"/>
-      <c r="I9" s="267"/>
-      <c r="J9" s="267"/>
-      <c r="K9" s="268"/>
+      <c r="E9" s="244"/>
+      <c r="F9" s="244"/>
+      <c r="G9" s="244"/>
+      <c r="H9" s="244"/>
+      <c r="I9" s="244"/>
+      <c r="J9" s="244"/>
+      <c r="K9" s="263"/>
       <c r="L9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M9" s="271" t="s">
+      <c r="M9" s="246" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="267"/>
-      <c r="O9" s="270"/>
+      <c r="N9" s="244"/>
+      <c r="O9" s="245"/>
     </row>
     <row r="10" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="257"/>
-      <c r="B10" s="258"/>
-      <c r="C10" s="259"/>
-      <c r="D10" s="275" t="s">
+      <c r="A10" s="273"/>
+      <c r="B10" s="248"/>
+      <c r="C10" s="249"/>
+      <c r="D10" s="247" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="258"/>
-      <c r="F10" s="258"/>
-      <c r="G10" s="258"/>
-      <c r="H10" s="258"/>
-      <c r="I10" s="258"/>
-      <c r="J10" s="258"/>
-      <c r="K10" s="259"/>
+      <c r="E10" s="248"/>
+      <c r="F10" s="248"/>
+      <c r="G10" s="248"/>
+      <c r="H10" s="248"/>
+      <c r="I10" s="248"/>
+      <c r="J10" s="248"/>
+      <c r="K10" s="249"/>
       <c r="L10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="271" t="s">
+      <c r="M10" s="246" t="s">
         <v>24</v>
       </c>
-      <c r="N10" s="267"/>
-      <c r="O10" s="270"/>
+      <c r="N10" s="244"/>
+      <c r="O10" s="245"/>
     </row>
     <row r="11" spans="1:15" ht="26" x14ac:dyDescent="0.25">
-      <c r="A11" s="251" t="s">
+      <c r="A11" s="250" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="252"/>
-      <c r="C11" s="253"/>
+      <c r="B11" s="251"/>
+      <c r="C11" s="252"/>
       <c r="D11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="279" t="s">
+      <c r="E11" s="259" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="264"/>
-      <c r="G11" s="264"/>
-      <c r="H11" s="264"/>
-      <c r="I11" s="264"/>
-      <c r="J11" s="264"/>
-      <c r="K11" s="264"/>
-      <c r="L11" s="264"/>
-      <c r="M11" s="264"/>
-      <c r="N11" s="264"/>
-      <c r="O11" s="265"/>
+      <c r="F11" s="260"/>
+      <c r="G11" s="260"/>
+      <c r="H11" s="260"/>
+      <c r="I11" s="260"/>
+      <c r="J11" s="260"/>
+      <c r="K11" s="260"/>
+      <c r="L11" s="260"/>
+      <c r="M11" s="260"/>
+      <c r="N11" s="260"/>
+      <c r="O11" s="261"/>
     </row>
     <row r="12" spans="1:15" ht="26" x14ac:dyDescent="0.25">
-      <c r="A12" s="254"/>
-      <c r="B12" s="255"/>
-      <c r="C12" s="256"/>
+      <c r="A12" s="253"/>
+      <c r="B12" s="254"/>
+      <c r="C12" s="255"/>
       <c r="D12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="280" t="s">
+      <c r="E12" s="262" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="267"/>
-      <c r="G12" s="267"/>
-      <c r="H12" s="267"/>
-      <c r="I12" s="267"/>
-      <c r="J12" s="267"/>
-      <c r="K12" s="267"/>
-      <c r="L12" s="267"/>
-      <c r="M12" s="267"/>
-      <c r="N12" s="267"/>
-      <c r="O12" s="270"/>
+      <c r="F12" s="244"/>
+      <c r="G12" s="244"/>
+      <c r="H12" s="244"/>
+      <c r="I12" s="244"/>
+      <c r="J12" s="244"/>
+      <c r="K12" s="244"/>
+      <c r="L12" s="244"/>
+      <c r="M12" s="244"/>
+      <c r="N12" s="244"/>
+      <c r="O12" s="245"/>
     </row>
     <row r="13" spans="1:15" ht="26" x14ac:dyDescent="0.25">
-      <c r="A13" s="254"/>
-      <c r="B13" s="255"/>
-      <c r="C13" s="256"/>
+      <c r="A13" s="253"/>
+      <c r="B13" s="254"/>
+      <c r="C13" s="255"/>
       <c r="D13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="280" t="s">
+      <c r="E13" s="262" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="267"/>
-      <c r="G13" s="268"/>
+      <c r="F13" s="244"/>
+      <c r="G13" s="263"/>
       <c r="H13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="280" t="s">
+      <c r="I13" s="262" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="267"/>
-      <c r="K13" s="268"/>
+      <c r="J13" s="244"/>
+      <c r="K13" s="263"/>
       <c r="L13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M13" s="280" t="s">
+      <c r="M13" s="262" t="s">
         <v>35</v>
       </c>
-      <c r="N13" s="267"/>
-      <c r="O13" s="270"/>
+      <c r="N13" s="244"/>
+      <c r="O13" s="245"/>
     </row>
     <row r="14" spans="1:15" ht="13" x14ac:dyDescent="0.25">
-      <c r="A14" s="254"/>
-      <c r="B14" s="255"/>
-      <c r="C14" s="256"/>
+      <c r="A14" s="253"/>
+      <c r="B14" s="254"/>
+      <c r="C14" s="255"/>
       <c r="D14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="271" t="s">
+      <c r="E14" s="246" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="267"/>
-      <c r="G14" s="267"/>
-      <c r="H14" s="267"/>
-      <c r="I14" s="267"/>
-      <c r="J14" s="267"/>
-      <c r="K14" s="267"/>
-      <c r="L14" s="267"/>
-      <c r="M14" s="267"/>
-      <c r="N14" s="267"/>
-      <c r="O14" s="270"/>
+      <c r="F14" s="244"/>
+      <c r="G14" s="244"/>
+      <c r="H14" s="244"/>
+      <c r="I14" s="244"/>
+      <c r="J14" s="244"/>
+      <c r="K14" s="244"/>
+      <c r="L14" s="244"/>
+      <c r="M14" s="244"/>
+      <c r="N14" s="244"/>
+      <c r="O14" s="245"/>
     </row>
     <row r="15" spans="1:15" ht="26" x14ac:dyDescent="0.25">
-      <c r="A15" s="254"/>
-      <c r="B15" s="255"/>
-      <c r="C15" s="256"/>
+      <c r="A15" s="253"/>
+      <c r="B15" s="254"/>
+      <c r="C15" s="255"/>
       <c r="D15" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="286"/>
-      <c r="F15" s="267"/>
-      <c r="G15" s="267"/>
-      <c r="H15" s="267"/>
-      <c r="I15" s="267"/>
-      <c r="J15" s="267"/>
-      <c r="K15" s="268"/>
+      <c r="E15" s="269"/>
+      <c r="F15" s="244"/>
+      <c r="G15" s="244"/>
+      <c r="H15" s="244"/>
+      <c r="I15" s="244"/>
+      <c r="J15" s="244"/>
+      <c r="K15" s="263"/>
       <c r="L15" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="M15" s="287"/>
-      <c r="N15" s="267"/>
-      <c r="O15" s="270"/>
+      <c r="M15" s="270"/>
+      <c r="N15" s="244"/>
+      <c r="O15" s="245"/>
     </row>
     <row r="16" spans="1:15" ht="26" x14ac:dyDescent="0.25">
-      <c r="A16" s="254"/>
-      <c r="B16" s="255"/>
-      <c r="C16" s="256"/>
+      <c r="A16" s="253"/>
+      <c r="B16" s="254"/>
+      <c r="C16" s="255"/>
       <c r="D16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="287" t="s">
+      <c r="E16" s="270" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="267"/>
-      <c r="G16" s="267"/>
-      <c r="H16" s="267"/>
-      <c r="I16" s="267"/>
-      <c r="J16" s="267"/>
-      <c r="K16" s="268"/>
+      <c r="F16" s="244"/>
+      <c r="G16" s="244"/>
+      <c r="H16" s="244"/>
+      <c r="I16" s="244"/>
+      <c r="J16" s="244"/>
+      <c r="K16" s="263"/>
       <c r="L16" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M16" s="280"/>
-      <c r="N16" s="267"/>
-      <c r="O16" s="270"/>
+      <c r="M16" s="262"/>
+      <c r="N16" s="244"/>
+      <c r="O16" s="245"/>
     </row>
     <row r="17" spans="1:15" ht="13" x14ac:dyDescent="0.25">
-      <c r="A17" s="254"/>
-      <c r="B17" s="255"/>
-      <c r="C17" s="256"/>
+      <c r="A17" s="253"/>
+      <c r="B17" s="254"/>
+      <c r="C17" s="255"/>
       <c r="D17" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="288"/>
-      <c r="F17" s="267"/>
-      <c r="G17" s="267"/>
-      <c r="H17" s="267"/>
-      <c r="I17" s="267"/>
-      <c r="J17" s="267"/>
-      <c r="K17" s="267"/>
-      <c r="L17" s="267"/>
-      <c r="M17" s="267"/>
-      <c r="N17" s="267"/>
-      <c r="O17" s="270"/>
+      <c r="E17" s="243"/>
+      <c r="F17" s="244"/>
+      <c r="G17" s="244"/>
+      <c r="H17" s="244"/>
+      <c r="I17" s="244"/>
+      <c r="J17" s="244"/>
+      <c r="K17" s="244"/>
+      <c r="L17" s="244"/>
+      <c r="M17" s="244"/>
+      <c r="N17" s="244"/>
+      <c r="O17" s="245"/>
     </row>
     <row r="18" spans="1:15" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="276"/>
-      <c r="B18" s="277"/>
-      <c r="C18" s="278"/>
+      <c r="A18" s="256"/>
+      <c r="B18" s="257"/>
+      <c r="C18" s="258"/>
       <c r="D18" s="8" t="s">
         <v>44</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="281"/>
-      <c r="G18" s="282"/>
-      <c r="H18" s="282"/>
-      <c r="I18" s="283"/>
-      <c r="J18" s="284" t="s">
+      <c r="F18" s="264"/>
+      <c r="G18" s="265"/>
+      <c r="H18" s="265"/>
+      <c r="I18" s="266"/>
+      <c r="J18" s="267" t="s">
         <v>46</v>
       </c>
-      <c r="K18" s="282"/>
-      <c r="L18" s="282"/>
-      <c r="M18" s="282"/>
-      <c r="N18" s="282"/>
-      <c r="O18" s="285"/>
+      <c r="K18" s="265"/>
+      <c r="L18" s="265"/>
+      <c r="M18" s="265"/>
+      <c r="N18" s="265"/>
+      <c r="O18" s="268"/>
     </row>
     <row r="19" spans="1:15" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="D9:K9"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:O2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:O3"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="A5:C10"/>
+    <mergeCell ref="D5:K5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="D6:K6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="D7:K7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="D8:K8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="L4:M4"/>
     <mergeCell ref="E17:O17"/>
     <mergeCell ref="M9:O9"/>
     <mergeCell ref="D10:K10"/>
@@ -13416,28 +13438,6 @@
     <mergeCell ref="E15:K15"/>
     <mergeCell ref="M15:O15"/>
     <mergeCell ref="E16:K16"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="A5:C10"/>
-    <mergeCell ref="D5:K5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="D6:K6"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="D7:K7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="D8:K8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="D9:K9"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:O2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:O3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M5" r:id="rId1" xr:uid="{DF32E119-BCC2-4DA3-96F6-DF2BC46B1D7F}"/>
@@ -22954,8 +22954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C943FC3-6890-431D-8DC7-652A117AB527}">
   <dimension ref="A1:B955"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -23861,32 +23861,32 @@
       </c>
     </row>
     <row r="113" spans="1:2" ht="14" x14ac:dyDescent="0.25">
-      <c r="A113" s="234">
-        <v>10503</v>
+      <c r="A113" s="234" t="s">
+        <v>316</v>
       </c>
       <c r="B113" s="235" t="s">
         <v>889</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="14" x14ac:dyDescent="0.25">
-      <c r="A114" s="234">
-        <v>10503</v>
+      <c r="A114" s="234" t="s">
+        <v>316</v>
       </c>
       <c r="B114" s="235" t="s">
         <v>891</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="14" x14ac:dyDescent="0.25">
-      <c r="A115" s="234">
-        <v>10503</v>
+      <c r="A115" s="234" t="s">
+        <v>316</v>
       </c>
       <c r="B115" s="235" t="s">
         <v>893</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="14" x14ac:dyDescent="0.25">
-      <c r="A116" s="234">
-        <v>10503</v>
+      <c r="A116" s="234" t="s">
+        <v>316</v>
       </c>
       <c r="B116" s="235" t="s">
         <v>900</v>
@@ -30808,7 +30808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D1F5C3-17E9-41F3-80D7-4A0448D85751}">
   <dimension ref="A1:E916"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A896" workbookViewId="0">
+    <sheetView topLeftCell="A896" workbookViewId="0">
       <selection activeCell="B914" sqref="B914"/>
     </sheetView>
   </sheetViews>
@@ -44461,435 +44461,460 @@
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" ht="126.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="290"/>
-      <c r="B1" s="291"/>
-      <c r="C1" s="291"/>
-      <c r="D1" s="291"/>
-      <c r="E1" s="291"/>
-      <c r="F1" s="291"/>
-      <c r="G1" s="291"/>
-      <c r="H1" s="291"/>
-      <c r="I1" s="291"/>
-      <c r="J1" s="291"/>
-      <c r="K1" s="291"/>
-      <c r="L1" s="291"/>
-      <c r="M1" s="291"/>
-      <c r="N1" s="291"/>
-      <c r="O1" s="292"/>
+      <c r="A1" s="309"/>
+      <c r="B1" s="310"/>
+      <c r="C1" s="310"/>
+      <c r="D1" s="310"/>
+      <c r="E1" s="310"/>
+      <c r="F1" s="310"/>
+      <c r="G1" s="310"/>
+      <c r="H1" s="310"/>
+      <c r="I1" s="310"/>
+      <c r="J1" s="310"/>
+      <c r="K1" s="310"/>
+      <c r="L1" s="310"/>
+      <c r="M1" s="310"/>
+      <c r="N1" s="310"/>
+      <c r="O1" s="311"/>
     </row>
     <row r="2" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="293" t="s">
+      <c r="A2" s="312" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="244"/>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
-      <c r="H2" s="244"/>
-      <c r="I2" s="244"/>
-      <c r="J2" s="244"/>
-      <c r="K2" s="244"/>
-      <c r="L2" s="244"/>
-      <c r="M2" s="244"/>
-      <c r="N2" s="244"/>
-      <c r="O2" s="245"/>
+      <c r="B2" s="281"/>
+      <c r="C2" s="281"/>
+      <c r="D2" s="281"/>
+      <c r="E2" s="281"/>
+      <c r="F2" s="281"/>
+      <c r="G2" s="281"/>
+      <c r="H2" s="281"/>
+      <c r="I2" s="281"/>
+      <c r="J2" s="281"/>
+      <c r="K2" s="281"/>
+      <c r="L2" s="281"/>
+      <c r="M2" s="281"/>
+      <c r="N2" s="281"/>
+      <c r="O2" s="272"/>
     </row>
     <row r="3" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="294" t="s">
+      <c r="A3" s="313" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="244"/>
-      <c r="C3" s="295"/>
-      <c r="D3" s="296" t="s">
+      <c r="B3" s="281"/>
+      <c r="C3" s="314"/>
+      <c r="D3" s="315" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="244"/>
-      <c r="F3" s="244"/>
-      <c r="G3" s="244"/>
-      <c r="H3" s="244"/>
-      <c r="I3" s="244"/>
-      <c r="J3" s="244"/>
-      <c r="K3" s="244"/>
-      <c r="L3" s="244"/>
-      <c r="M3" s="244"/>
-      <c r="N3" s="244"/>
-      <c r="O3" s="245"/>
+      <c r="E3" s="281"/>
+      <c r="F3" s="281"/>
+      <c r="G3" s="281"/>
+      <c r="H3" s="281"/>
+      <c r="I3" s="281"/>
+      <c r="J3" s="281"/>
+      <c r="K3" s="281"/>
+      <c r="L3" s="281"/>
+      <c r="M3" s="281"/>
+      <c r="N3" s="281"/>
+      <c r="O3" s="272"/>
     </row>
     <row r="4" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="294" t="s">
+      <c r="A4" s="313" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="244"/>
-      <c r="C4" s="295"/>
-      <c r="D4" s="297" t="s">
+      <c r="B4" s="281"/>
+      <c r="C4" s="314"/>
+      <c r="D4" s="316" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="244"/>
-      <c r="F4" s="244"/>
-      <c r="G4" s="244"/>
-      <c r="H4" s="244"/>
-      <c r="I4" s="244"/>
-      <c r="J4" s="244"/>
-      <c r="K4" s="244"/>
-      <c r="L4" s="244"/>
-      <c r="M4" s="244"/>
-      <c r="N4" s="244"/>
-      <c r="O4" s="245"/>
+      <c r="E4" s="281"/>
+      <c r="F4" s="281"/>
+      <c r="G4" s="281"/>
+      <c r="H4" s="281"/>
+      <c r="I4" s="281"/>
+      <c r="J4" s="281"/>
+      <c r="K4" s="281"/>
+      <c r="L4" s="281"/>
+      <c r="M4" s="281"/>
+      <c r="N4" s="281"/>
+      <c r="O4" s="272"/>
     </row>
     <row r="5" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="294" t="s">
+      <c r="A5" s="313" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="244"/>
-      <c r="C5" s="295"/>
-      <c r="D5" s="298" t="s">
+      <c r="B5" s="281"/>
+      <c r="C5" s="314"/>
+      <c r="D5" s="317" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="244"/>
-      <c r="F5" s="295"/>
-      <c r="G5" s="299" t="s">
+      <c r="E5" s="281"/>
+      <c r="F5" s="314"/>
+      <c r="G5" s="318" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="295"/>
-      <c r="I5" s="300" t="s">
+      <c r="H5" s="314"/>
+      <c r="I5" s="319" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="244"/>
-      <c r="K5" s="295"/>
-      <c r="L5" s="299" t="s">
+      <c r="J5" s="281"/>
+      <c r="K5" s="314"/>
+      <c r="L5" s="318" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="295"/>
-      <c r="N5" s="289" t="s">
+      <c r="M5" s="314"/>
+      <c r="N5" s="308" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="245"/>
+      <c r="O5" s="272"/>
     </row>
     <row r="6" spans="1:15" ht="13" x14ac:dyDescent="0.25">
-      <c r="A6" s="301" t="s">
+      <c r="A6" s="289" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="302"/>
-      <c r="C6" s="303"/>
-      <c r="D6" s="307" t="s">
+      <c r="B6" s="290"/>
+      <c r="C6" s="291"/>
+      <c r="D6" s="304" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="261"/>
-      <c r="F6" s="261"/>
-      <c r="G6" s="261"/>
-      <c r="H6" s="261"/>
-      <c r="I6" s="261"/>
-      <c r="J6" s="261"/>
-      <c r="K6" s="308"/>
+      <c r="E6" s="275"/>
+      <c r="F6" s="275"/>
+      <c r="G6" s="275"/>
+      <c r="H6" s="275"/>
+      <c r="I6" s="275"/>
+      <c r="J6" s="275"/>
+      <c r="K6" s="305"/>
       <c r="L6" s="205" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="263" t="s">
+      <c r="M6" s="277" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="264"/>
-      <c r="O6" s="265"/>
+      <c r="N6" s="260"/>
+      <c r="O6" s="261"/>
     </row>
     <row r="7" spans="1:15" ht="13" x14ac:dyDescent="0.25">
-      <c r="A7" s="304"/>
-      <c r="B7" s="255"/>
-      <c r="C7" s="305"/>
-      <c r="D7" s="309" t="s">
+      <c r="A7" s="292"/>
+      <c r="B7" s="254"/>
+      <c r="C7" s="293"/>
+      <c r="D7" s="306" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="267"/>
-      <c r="F7" s="267"/>
-      <c r="G7" s="267"/>
-      <c r="H7" s="267"/>
-      <c r="I7" s="267"/>
-      <c r="J7" s="267"/>
-      <c r="K7" s="310"/>
+      <c r="E7" s="244"/>
+      <c r="F7" s="244"/>
+      <c r="G7" s="244"/>
+      <c r="H7" s="244"/>
+      <c r="I7" s="244"/>
+      <c r="J7" s="244"/>
+      <c r="K7" s="297"/>
       <c r="L7" s="206" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="311" t="s">
+      <c r="M7" s="307" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="267"/>
-      <c r="O7" s="270"/>
+      <c r="N7" s="244"/>
+      <c r="O7" s="245"/>
     </row>
     <row r="8" spans="1:15" ht="13" x14ac:dyDescent="0.25">
-      <c r="A8" s="304"/>
-      <c r="B8" s="255"/>
-      <c r="C8" s="305"/>
-      <c r="D8" s="309" t="s">
+      <c r="A8" s="292"/>
+      <c r="B8" s="254"/>
+      <c r="C8" s="293"/>
+      <c r="D8" s="306" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="267"/>
-      <c r="F8" s="267"/>
-      <c r="G8" s="267"/>
-      <c r="H8" s="267"/>
-      <c r="I8" s="267"/>
-      <c r="J8" s="267"/>
-      <c r="K8" s="310"/>
+      <c r="E8" s="244"/>
+      <c r="F8" s="244"/>
+      <c r="G8" s="244"/>
+      <c r="H8" s="244"/>
+      <c r="I8" s="244"/>
+      <c r="J8" s="244"/>
+      <c r="K8" s="297"/>
       <c r="L8" s="206" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="312" t="s">
+      <c r="M8" s="298" t="s">
         <v>18</v>
       </c>
-      <c r="N8" s="267"/>
-      <c r="O8" s="270"/>
+      <c r="N8" s="244"/>
+      <c r="O8" s="245"/>
     </row>
     <row r="9" spans="1:15" ht="13" x14ac:dyDescent="0.25">
-      <c r="A9" s="304"/>
-      <c r="B9" s="255"/>
-      <c r="C9" s="305"/>
-      <c r="D9" s="309" t="s">
+      <c r="A9" s="292"/>
+      <c r="B9" s="254"/>
+      <c r="C9" s="293"/>
+      <c r="D9" s="306" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="267"/>
-      <c r="F9" s="267"/>
-      <c r="G9" s="267"/>
-      <c r="H9" s="267"/>
-      <c r="I9" s="267"/>
-      <c r="J9" s="267"/>
-      <c r="K9" s="310"/>
+      <c r="E9" s="244"/>
+      <c r="F9" s="244"/>
+      <c r="G9" s="244"/>
+      <c r="H9" s="244"/>
+      <c r="I9" s="244"/>
+      <c r="J9" s="244"/>
+      <c r="K9" s="297"/>
       <c r="L9" s="207" t="s">
         <v>13</v>
       </c>
-      <c r="M9" s="311" t="s">
+      <c r="M9" s="307" t="s">
         <v>20</v>
       </c>
-      <c r="N9" s="267"/>
-      <c r="O9" s="270"/>
+      <c r="N9" s="244"/>
+      <c r="O9" s="245"/>
     </row>
     <row r="10" spans="1:15" ht="13" x14ac:dyDescent="0.25">
-      <c r="A10" s="304"/>
-      <c r="B10" s="255"/>
-      <c r="C10" s="305"/>
-      <c r="D10" s="309" t="s">
+      <c r="A10" s="292"/>
+      <c r="B10" s="254"/>
+      <c r="C10" s="293"/>
+      <c r="D10" s="306" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="267"/>
-      <c r="F10" s="267"/>
-      <c r="G10" s="267"/>
-      <c r="H10" s="267"/>
-      <c r="I10" s="267"/>
-      <c r="J10" s="267"/>
-      <c r="K10" s="310"/>
+      <c r="E10" s="244"/>
+      <c r="F10" s="244"/>
+      <c r="G10" s="244"/>
+      <c r="H10" s="244"/>
+      <c r="I10" s="244"/>
+      <c r="J10" s="244"/>
+      <c r="K10" s="297"/>
       <c r="L10" s="207" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="312" t="s">
+      <c r="M10" s="298" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="267"/>
-      <c r="O10" s="270"/>
+      <c r="N10" s="244"/>
+      <c r="O10" s="245"/>
     </row>
     <row r="11" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="257"/>
-      <c r="B11" s="258"/>
-      <c r="C11" s="306"/>
-      <c r="D11" s="275" t="s">
+      <c r="A11" s="273"/>
+      <c r="B11" s="248"/>
+      <c r="C11" s="303"/>
+      <c r="D11" s="247" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="258"/>
-      <c r="F11" s="258"/>
-      <c r="G11" s="258"/>
-      <c r="H11" s="258"/>
-      <c r="I11" s="258"/>
-      <c r="J11" s="258"/>
-      <c r="K11" s="306"/>
+      <c r="E11" s="248"/>
+      <c r="F11" s="248"/>
+      <c r="G11" s="248"/>
+      <c r="H11" s="248"/>
+      <c r="I11" s="248"/>
+      <c r="J11" s="248"/>
+      <c r="K11" s="303"/>
       <c r="L11" s="208" t="s">
         <v>13</v>
       </c>
-      <c r="M11" s="312" t="s">
+      <c r="M11" s="298" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="267"/>
-      <c r="O11" s="270"/>
+      <c r="N11" s="244"/>
+      <c r="O11" s="245"/>
     </row>
     <row r="12" spans="1:15" ht="26" x14ac:dyDescent="0.25">
-      <c r="A12" s="301" t="s">
+      <c r="A12" s="289" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="302"/>
-      <c r="C12" s="303"/>
+      <c r="B12" s="290"/>
+      <c r="C12" s="291"/>
       <c r="D12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="279" t="s">
+      <c r="E12" s="259" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="264"/>
-      <c r="G12" s="264"/>
-      <c r="H12" s="264"/>
-      <c r="I12" s="264"/>
-      <c r="J12" s="264"/>
-      <c r="K12" s="264"/>
-      <c r="L12" s="264"/>
-      <c r="M12" s="264"/>
-      <c r="N12" s="264"/>
-      <c r="O12" s="265"/>
+      <c r="F12" s="260"/>
+      <c r="G12" s="260"/>
+      <c r="H12" s="260"/>
+      <c r="I12" s="260"/>
+      <c r="J12" s="260"/>
+      <c r="K12" s="260"/>
+      <c r="L12" s="260"/>
+      <c r="M12" s="260"/>
+      <c r="N12" s="260"/>
+      <c r="O12" s="261"/>
     </row>
     <row r="13" spans="1:15" ht="26" x14ac:dyDescent="0.25">
-      <c r="A13" s="304"/>
-      <c r="B13" s="255"/>
-      <c r="C13" s="305"/>
+      <c r="A13" s="292"/>
+      <c r="B13" s="254"/>
+      <c r="C13" s="293"/>
       <c r="D13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="315" t="s">
+      <c r="E13" s="296" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="267"/>
-      <c r="G13" s="267"/>
-      <c r="H13" s="267"/>
-      <c r="I13" s="267"/>
-      <c r="J13" s="267"/>
-      <c r="K13" s="267"/>
-      <c r="L13" s="267"/>
-      <c r="M13" s="267"/>
-      <c r="N13" s="267"/>
-      <c r="O13" s="270"/>
+      <c r="F13" s="244"/>
+      <c r="G13" s="244"/>
+      <c r="H13" s="244"/>
+      <c r="I13" s="244"/>
+      <c r="J13" s="244"/>
+      <c r="K13" s="244"/>
+      <c r="L13" s="244"/>
+      <c r="M13" s="244"/>
+      <c r="N13" s="244"/>
+      <c r="O13" s="245"/>
     </row>
     <row r="14" spans="1:15" ht="26" x14ac:dyDescent="0.25">
-      <c r="A14" s="304"/>
-      <c r="B14" s="255"/>
-      <c r="C14" s="305"/>
+      <c r="A14" s="292"/>
+      <c r="B14" s="254"/>
+      <c r="C14" s="293"/>
       <c r="D14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="315" t="s">
+      <c r="E14" s="296" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="267"/>
-      <c r="G14" s="310"/>
+      <c r="F14" s="244"/>
+      <c r="G14" s="297"/>
       <c r="H14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="315" t="s">
+      <c r="I14" s="296" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="267"/>
-      <c r="K14" s="310"/>
+      <c r="J14" s="244"/>
+      <c r="K14" s="297"/>
       <c r="L14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M14" s="315" t="s">
+      <c r="M14" s="296" t="s">
         <v>35</v>
       </c>
-      <c r="N14" s="267"/>
-      <c r="O14" s="270"/>
+      <c r="N14" s="244"/>
+      <c r="O14" s="245"/>
     </row>
     <row r="15" spans="1:15" ht="13" x14ac:dyDescent="0.25">
-      <c r="A15" s="304"/>
-      <c r="B15" s="255"/>
-      <c r="C15" s="305"/>
+      <c r="A15" s="292"/>
+      <c r="B15" s="254"/>
+      <c r="C15" s="293"/>
       <c r="D15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="312" t="s">
+      <c r="E15" s="298" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="267"/>
-      <c r="G15" s="267"/>
-      <c r="H15" s="267"/>
-      <c r="I15" s="267"/>
-      <c r="J15" s="267"/>
-      <c r="K15" s="267"/>
-      <c r="L15" s="267"/>
-      <c r="M15" s="267"/>
-      <c r="N15" s="267"/>
-      <c r="O15" s="270"/>
+      <c r="F15" s="244"/>
+      <c r="G15" s="244"/>
+      <c r="H15" s="244"/>
+      <c r="I15" s="244"/>
+      <c r="J15" s="244"/>
+      <c r="K15" s="244"/>
+      <c r="L15" s="244"/>
+      <c r="M15" s="244"/>
+      <c r="N15" s="244"/>
+      <c r="O15" s="245"/>
     </row>
     <row r="16" spans="1:15" ht="26" x14ac:dyDescent="0.25">
-      <c r="A16" s="304"/>
-      <c r="B16" s="255"/>
-      <c r="C16" s="305"/>
+      <c r="A16" s="292"/>
+      <c r="B16" s="254"/>
+      <c r="C16" s="293"/>
       <c r="D16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="317"/>
-      <c r="F16" s="267"/>
-      <c r="G16" s="267"/>
-      <c r="H16" s="267"/>
-      <c r="I16" s="267"/>
-      <c r="J16" s="267"/>
-      <c r="K16" s="310"/>
+      <c r="E16" s="300"/>
+      <c r="F16" s="244"/>
+      <c r="G16" s="244"/>
+      <c r="H16" s="244"/>
+      <c r="I16" s="244"/>
+      <c r="J16" s="244"/>
+      <c r="K16" s="297"/>
       <c r="L16" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="M16" s="318"/>
-      <c r="N16" s="267"/>
-      <c r="O16" s="270"/>
+      <c r="M16" s="301"/>
+      <c r="N16" s="244"/>
+      <c r="O16" s="245"/>
     </row>
     <row r="17" spans="1:15" ht="26" x14ac:dyDescent="0.25">
-      <c r="A17" s="304"/>
-      <c r="B17" s="255"/>
-      <c r="C17" s="305"/>
+      <c r="A17" s="292"/>
+      <c r="B17" s="254"/>
+      <c r="C17" s="293"/>
       <c r="D17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="318" t="s">
+      <c r="E17" s="301" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="267"/>
-      <c r="G17" s="267"/>
-      <c r="H17" s="267"/>
-      <c r="I17" s="267"/>
-      <c r="J17" s="267"/>
-      <c r="K17" s="310"/>
+      <c r="F17" s="244"/>
+      <c r="G17" s="244"/>
+      <c r="H17" s="244"/>
+      <c r="I17" s="244"/>
+      <c r="J17" s="244"/>
+      <c r="K17" s="297"/>
       <c r="L17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M17" s="315"/>
-      <c r="N17" s="267"/>
-      <c r="O17" s="270"/>
+      <c r="M17" s="296"/>
+      <c r="N17" s="244"/>
+      <c r="O17" s="245"/>
     </row>
     <row r="18" spans="1:15" ht="13" x14ac:dyDescent="0.25">
-      <c r="A18" s="304"/>
-      <c r="B18" s="255"/>
-      <c r="C18" s="305"/>
+      <c r="A18" s="292"/>
+      <c r="B18" s="254"/>
+      <c r="C18" s="293"/>
       <c r="D18" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="319"/>
-      <c r="F18" s="267"/>
-      <c r="G18" s="267"/>
-      <c r="H18" s="267"/>
-      <c r="I18" s="267"/>
-      <c r="J18" s="267"/>
-      <c r="K18" s="267"/>
-      <c r="L18" s="267"/>
-      <c r="M18" s="267"/>
-      <c r="N18" s="267"/>
-      <c r="O18" s="270"/>
+      <c r="E18" s="302"/>
+      <c r="F18" s="244"/>
+      <c r="G18" s="244"/>
+      <c r="H18" s="244"/>
+      <c r="I18" s="244"/>
+      <c r="J18" s="244"/>
+      <c r="K18" s="244"/>
+      <c r="L18" s="244"/>
+      <c r="M18" s="244"/>
+      <c r="N18" s="244"/>
+      <c r="O18" s="245"/>
     </row>
     <row r="19" spans="1:15" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="313"/>
-      <c r="B19" s="314"/>
-      <c r="C19" s="278"/>
+      <c r="A19" s="294"/>
+      <c r="B19" s="295"/>
+      <c r="C19" s="258"/>
       <c r="D19" s="8" t="s">
         <v>44</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="281"/>
-      <c r="G19" s="282"/>
-      <c r="H19" s="282"/>
-      <c r="I19" s="316"/>
-      <c r="J19" s="284" t="s">
+      <c r="F19" s="264"/>
+      <c r="G19" s="265"/>
+      <c r="H19" s="265"/>
+      <c r="I19" s="299"/>
+      <c r="J19" s="267" t="s">
         <v>46</v>
       </c>
-      <c r="K19" s="282"/>
-      <c r="L19" s="282"/>
-      <c r="M19" s="282"/>
-      <c r="N19" s="282"/>
-      <c r="O19" s="285"/>
+      <c r="K19" s="265"/>
+      <c r="L19" s="265"/>
+      <c r="M19" s="265"/>
+      <c r="N19" s="265"/>
+      <c r="O19" s="268"/>
     </row>
     <row r="20" spans="1:15" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:O3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:O4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="A6:C11"/>
+    <mergeCell ref="D6:K6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="D7:K7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="D8:K8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="D9:K9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="D10:K10"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="D11:K11"/>
+    <mergeCell ref="M11:O11"/>
     <mergeCell ref="A12:C19"/>
     <mergeCell ref="E12:O12"/>
     <mergeCell ref="E13:O13"/>
@@ -44904,31 +44929,6 @@
     <mergeCell ref="E17:K17"/>
     <mergeCell ref="M17:O17"/>
     <mergeCell ref="E18:O18"/>
-    <mergeCell ref="A6:C11"/>
-    <mergeCell ref="D6:K6"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="D7:K7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="D8:K8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="D9:K9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="D10:K10"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="D11:K11"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:O3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:O4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:M5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M6" r:id="rId1" xr:uid="{7137876C-A0D2-4A4A-AAEB-2159A1F2B40B}"/>

</xml_diff>